<commit_message>
added: Chisel and Bits SecurityCraft
</commit_message>
<xml_diff>
--- a/1.16.5_Modpack_client.xlsx
+++ b/1.16.5_Modpack_client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRNGX\curseforge\minecraft\Instances\The-1.16.5-Pack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7388EACE-FACD-48F3-8DB0-049C35356535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CF4EC9-FCD5-4778-8149-F4DB2E4952CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3210" yWindow="660" windowWidth="21600" windowHeight="11385" xr2:uid="{5855CEE6-8074-46FF-AC8E-288D8E80783C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="182">
   <si>
     <t>Installed:</t>
   </si>
@@ -265,18 +265,9 @@
     <t>Furnish</t>
   </si>
   <si>
-    <t>Infinit Dungeons</t>
-  </si>
-  <si>
-    <t>Soul Shard</t>
-  </si>
-  <si>
     <t>Cataclysm</t>
   </si>
   <si>
-    <t>Industrial Revolution</t>
-  </si>
-  <si>
     <t>Modular Powersuits</t>
   </si>
   <si>
@@ -364,9 +355,6 @@
     <t>BE</t>
   </si>
   <si>
-    <t>Only until Galacticraft is available</t>
-  </si>
-  <si>
     <t>Obfuscate</t>
   </si>
   <si>
@@ -562,7 +550,37 @@
     <t>5.5e</t>
   </si>
   <si>
-    <t>Micr+A44:K100ocosm</t>
+    <t>1.0.63</t>
+  </si>
+  <si>
+    <t>V: 0.0.1 | D: 08.04.22</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>Microcosm</t>
+  </si>
+  <si>
+    <t>1.9.1</t>
+  </si>
+  <si>
+    <t>1.4.1.3</t>
+  </si>
+  <si>
+    <t>Modloader</t>
+  </si>
+  <si>
+    <t>raplaced by galacticraft soon</t>
+  </si>
+  <si>
+    <t>2.2.18</t>
+  </si>
+  <si>
+    <t>36.2.20</t>
+  </si>
+  <si>
+    <t>Forge</t>
   </si>
 </sst>
 </file>
@@ -613,19 +631,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -643,15 +670,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D07528F-1E51-4ACA-8A46-9CBD097B5B3E}" name="Tabelle1" displayName="Tabelle1" ref="A1:K501" totalsRowShown="0">
-  <autoFilter ref="A1:K501" xr:uid="{5D07528F-1E51-4ACA-8A46-9CBD097B5B3E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K447">
-    <sortCondition ref="A1:A501"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D07528F-1E51-4ACA-8A46-9CBD097B5B3E}" name="Tabelle1" displayName="Tabelle1" ref="A1:K498" totalsRowShown="0">
+  <autoFilter ref="A1:K498" xr:uid="{5D07528F-1E51-4ACA-8A46-9CBD097B5B3E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K444">
+    <sortCondition ref="A1:A498"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{1747115B-0107-4CC6-BBBA-07CD5460D2C4}" name="Name:X"/>
-    <tableColumn id="2" xr3:uid="{CF86DC55-B297-46AE-A2AB-1C3DCE44D2AE}" name="Installed:"/>
-    <tableColumn id="12" xr3:uid="{018CFAA4-D3E8-4FB5-B3CD-FC76DAEF0A6B}" name="Version:" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{CF86DC55-B297-46AE-A2AB-1C3DCE44D2AE}" name="Installed:" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{018CFAA4-D3E8-4FB5-B3CD-FC76DAEF0A6B}" name="Version:" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{DBC3A8FE-FB7E-4CDA-83B7-143437351C2F}" name="Client  side:"/>
     <tableColumn id="4" xr3:uid="{3A1BACBD-2AD6-4896-9B6F-559725FE1D90}" name="Server  side:"/>
     <tableColumn id="5" xr3:uid="{AB217EB1-7BA6-4EAF-882F-7608700FCE01}" name="have a look at:"/>
@@ -962,16 +989,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4CD30AE-F806-4131-A40A-9F8A05DF208C}">
-  <dimension ref="A1:K447"/>
+  <dimension ref="A1:K444"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K75" sqref="K75"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="6"/>
     <col min="3" max="3" width="11.42578125" style="2"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
@@ -979,19 +1007,19 @@
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1006,7 +1034,7 @@
         <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I1" t="s">
         <v>32</v>
@@ -1015,98 +1043,98 @@
         <v>61</v>
       </c>
       <c r="K1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G2" t="s">
         <v>67</v>
       </c>
       <c r="H2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G3" t="s">
         <v>67</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G4" t="s">
         <v>67</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K5" t="s">
-        <v>109</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J6" t="s">
         <v>22</v>
@@ -1116,92 +1144,92 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G7" t="s">
         <v>67</v>
       </c>
       <c r="H7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G8" t="s">
         <v>67</v>
       </c>
       <c r="H8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G9" t="s">
         <v>67</v>
       </c>
       <c r="H9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B10" t="s">
-        <v>114</v>
+      <c r="B10" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G11" t="s">
         <v>67</v>
       </c>
       <c r="H11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F12" t="s">
@@ -1211,52 +1239,52 @@
         <v>67</v>
       </c>
       <c r="H12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G13" t="s">
         <v>67</v>
       </c>
       <c r="H13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" t="s">
-        <v>21</v>
+      <c r="B14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="G14" t="s">
-        <v>67</v>
+        <v>172</v>
       </c>
       <c r="H14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
@@ -1265,7 +1293,7 @@
         <v>68</v>
       </c>
       <c r="H15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J15" t="s">
         <v>22</v>
@@ -1275,81 +1303,81 @@
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G16" t="s">
         <v>67</v>
       </c>
       <c r="H16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B17" t="str">
-        <f>VLOOKUP("Ender Storage",$A$2:$B$495,2)</f>
+      <c r="B17" s="6" t="str">
+        <f>VLOOKUP("Ender Storage",$A$2:$B$492,2)</f>
         <v>Y</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G17" t="s">
         <v>67</v>
       </c>
       <c r="H17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B18" t="str">
-        <f>VLOOKUP("Thermal Foundation",$A$2:$B$495,2)</f>
+      <c r="B18" s="6" t="str">
+        <f>VLOOKUP("Thermal Foundation",$A$2:$B$492,2)</f>
         <v>Y</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G18" t="s">
         <v>67</v>
       </c>
       <c r="H18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G19" t="s">
         <v>67</v>
       </c>
       <c r="H19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1358,92 +1386,92 @@
         <v>67</v>
       </c>
       <c r="H20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G21" t="s">
         <v>67</v>
       </c>
       <c r="H21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G22" t="s">
         <v>67</v>
       </c>
       <c r="H22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
-        <v>114</v>
+      <c r="B23" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G23" t="s">
         <v>116</v>
       </c>
-      <c r="G23" t="s">
-        <v>120</v>
-      </c>
       <c r="H23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G24" t="s">
         <v>68</v>
       </c>
       <c r="H24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G25" t="s">
         <v>67</v>
       </c>
       <c r="H25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J25" t="s">
         <v>22</v>
@@ -1453,51 +1481,51 @@
       <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G26" t="s">
         <v>67</v>
       </c>
       <c r="H26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G27" t="s">
         <v>68</v>
       </c>
       <c r="H27" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G28" t="s">
         <v>68</v>
       </c>
       <c r="H28" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I28" t="s">
         <v>73</v>
@@ -1507,24 +1535,24 @@
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G29" t="s">
         <v>67</v>
       </c>
       <c r="H29" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F30" t="s">
@@ -1534,7 +1562,7 @@
         <v>67</v>
       </c>
       <c r="H30" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J30" t="s">
         <v>22</v>
@@ -1544,17 +1572,17 @@
       <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G31" t="s">
         <v>68</v>
       </c>
       <c r="H31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J31" t="s">
         <v>22</v>
@@ -1564,17 +1592,17 @@
       <c r="A32" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G32" t="s">
         <v>67</v>
       </c>
       <c r="H32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J32" t="s">
         <v>22</v>
@@ -1584,310 +1612,316 @@
       <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G33" t="s">
         <v>67</v>
       </c>
       <c r="H33" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G34" t="s">
         <v>67</v>
       </c>
       <c r="H34" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F35" t="s">
-        <v>21</v>
-      </c>
       <c r="G35" t="s">
         <v>67</v>
       </c>
       <c r="H35" t="s">
-        <v>93</v>
+        <v>82</v>
+      </c>
+      <c r="J35" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>76</v>
-      </c>
-      <c r="B36" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36" t="s">
-        <v>21</v>
+      <c r="A36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="G36" t="s">
         <v>67</v>
       </c>
       <c r="H36" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>112</v>
-      </c>
-      <c r="B37" t="s">
-        <v>26</v>
+      <c r="A37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="G37" t="s">
         <v>67</v>
       </c>
       <c r="H37" t="s">
-        <v>85</v>
-      </c>
-      <c r="J37" t="s">
-        <v>22</v>
+        <v>87</v>
+      </c>
+      <c r="I37" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="G38" t="s">
-        <v>67</v>
+        <v>172</v>
       </c>
       <c r="H38" t="s">
-        <v>90</v>
+        <v>87</v>
+      </c>
+      <c r="I38" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G39" t="s">
         <v>67</v>
       </c>
       <c r="H39" t="s">
-        <v>90</v>
-      </c>
-      <c r="I39" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" t="s">
-        <v>26</v>
+      <c r="A40" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="G40" t="s">
         <v>67</v>
       </c>
       <c r="H40" t="s">
-        <v>90</v>
-      </c>
-      <c r="I40" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G41" t="s">
-        <v>67</v>
-      </c>
-      <c r="H41" t="s">
-        <v>95</v>
-      </c>
+      <c r="A41" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="7" t="str">
+        <f>VLOOKUP("Tinkers Construct",$A$2:$B$492,2)</f>
+        <v>Y</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" t="s">
+        <v>174</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G42" t="s">
         <v>67</v>
       </c>
       <c r="H42" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="J42" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="4" t="str">
-        <f>VLOOKUP("Tinkers Construct",$A$2:$B$495,2)</f>
-        <v>Y</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
+      <c r="A43" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G43" t="s">
+        <v>172</v>
+      </c>
+      <c r="H43" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G44" t="s">
         <v>67</v>
       </c>
       <c r="H44" t="s">
-        <v>97</v>
-      </c>
-      <c r="J44" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F45" t="s">
-        <v>21</v>
-      </c>
       <c r="G45" t="s">
         <v>67</v>
       </c>
       <c r="H45" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" t="s">
-        <v>22</v>
+        <v>58</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="G46" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="H46" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B47" t="s">
-        <v>26</v>
+      <c r="A47" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="G47" t="s">
         <v>67</v>
       </c>
       <c r="H47" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48" t="s">
-        <v>114</v>
+        <v>56</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>117</v>
+        <v>137</v>
+      </c>
+      <c r="F48" t="s">
+        <v>21</v>
       </c>
       <c r="G48" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="H48" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G49" t="s">
         <v>67</v>
       </c>
       <c r="H49" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="J49" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50" t="s">
-        <v>22</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>141</v>
+      <c r="A50" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F50" t="s">
         <v>21</v>
@@ -1896,35 +1930,35 @@
         <v>67</v>
       </c>
       <c r="H50" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G51" t="s">
         <v>67</v>
       </c>
       <c r="H51" t="s">
-        <v>93</v>
-      </c>
-      <c r="J51" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>110</v>
-      </c>
-      <c r="B52" t="s">
-        <v>26</v>
+      <c r="A52" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="F52" t="s">
         <v>21</v>
@@ -1933,277 +1967,280 @@
         <v>67</v>
       </c>
       <c r="H52" t="s">
-        <v>85</v>
+        <v>96</v>
+      </c>
+      <c r="I52" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B53" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G53" t="s">
         <v>67</v>
       </c>
       <c r="H53" t="s">
-        <v>98</v>
+        <v>90</v>
+      </c>
+      <c r="J53" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F54" t="s">
+        <v>132</v>
+      </c>
+      <c r="G54" t="s">
+        <v>67</v>
+      </c>
+      <c r="H54" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" t="s">
+        <v>22</v>
+      </c>
+      <c r="F55" t="s">
         <v>21</v>
       </c>
-      <c r="G54" t="s">
-        <v>67</v>
-      </c>
-      <c r="H54" t="s">
-        <v>99</v>
-      </c>
-      <c r="I54" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B55" t="s">
-        <v>22</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="G55" t="s">
         <v>67</v>
       </c>
       <c r="H55" t="s">
-        <v>93</v>
-      </c>
-      <c r="J55" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B56" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G56" t="s">
         <v>67</v>
       </c>
       <c r="H56" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>41</v>
-      </c>
-      <c r="B57" t="s">
-        <v>26</v>
-      </c>
-      <c r="D57" t="s">
-        <v>22</v>
-      </c>
-      <c r="F57" t="s">
-        <v>21</v>
+      <c r="A57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="G57" t="s">
-        <v>67</v>
+        <v>172</v>
       </c>
       <c r="H57" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G58" t="s">
         <v>67</v>
       </c>
       <c r="H58" t="s">
-        <v>85</v>
+        <v>92</v>
+      </c>
+      <c r="J58" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" t="s">
-        <v>26</v>
-      </c>
-      <c r="F59" t="s">
-        <v>21</v>
+      <c r="A59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="G59" t="s">
         <v>67</v>
       </c>
       <c r="H59" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G60" t="s">
         <v>67</v>
       </c>
       <c r="H60" t="s">
-        <v>95</v>
-      </c>
-      <c r="J60" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>77</v>
-      </c>
-      <c r="B61" t="s">
-        <v>26</v>
-      </c>
-      <c r="F61" t="s">
-        <v>21</v>
+      <c r="A61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="G61" t="s">
         <v>67</v>
       </c>
       <c r="H61" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B62" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G62" t="s">
         <v>67</v>
       </c>
       <c r="H62" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B63" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>132</v>
+        <v>176</v>
       </c>
       <c r="G63" t="s">
-        <v>67</v>
+        <v>172</v>
       </c>
       <c r="H63" t="s">
-        <v>85</v>
+        <v>90</v>
+      </c>
+      <c r="I63" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G64" t="s">
         <v>67</v>
       </c>
       <c r="H64" t="s">
-        <v>85</v>
+        <v>90</v>
+      </c>
+      <c r="I64" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G65" t="s">
         <v>67</v>
       </c>
       <c r="H65" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>36</v>
-      </c>
-      <c r="B66" t="s">
-        <v>26</v>
+      <c r="A66" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="G66" t="s">
         <v>67</v>
       </c>
       <c r="H66" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I66" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B67" t="s">
-        <v>22</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>129</v>
+      <c r="A67" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="G67" t="s">
         <v>67</v>
       </c>
       <c r="H67" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I67" t="s">
         <v>65</v>
@@ -2211,155 +2248,131 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B68" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G68" t="s">
         <v>67</v>
       </c>
       <c r="H68" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>34</v>
-      </c>
-      <c r="B69" t="s">
-        <v>26</v>
+      <c r="A69" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="G69" t="s">
         <v>67</v>
       </c>
       <c r="H69" t="s">
-        <v>93</v>
-      </c>
-      <c r="I69" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>35</v>
-      </c>
-      <c r="B70" t="s">
-        <v>26</v>
+      <c r="A70" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="G70" t="s">
         <v>67</v>
       </c>
       <c r="H70" t="s">
-        <v>93</v>
-      </c>
-      <c r="I70" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B71" t="s">
+        <v>64</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G71" t="s">
         <v>67</v>
       </c>
       <c r="H71" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B72" t="s">
+        <v>54</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G72" t="s">
         <v>67</v>
       </c>
       <c r="H72" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B73" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="G73" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H73" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B74" t="s">
+      <c r="A74" t="s">
+        <v>181</v>
+      </c>
+      <c r="B74" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>124</v>
+        <v>180</v>
       </c>
       <c r="G74" t="s">
         <v>67</v>
       </c>
       <c r="H74" t="s">
-        <v>101</v>
+        <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B75" t="s">
-        <v>22</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="G75" t="s">
         <v>67</v>
       </c>
-      <c r="H75" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B76" t="s">
-        <v>22</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="G76" t="s">
-        <v>68</v>
-      </c>
-      <c r="H76" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -4199,59 +4212,44 @@
     </row>
     <row r="444" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G444" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="445" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G445" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="446" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G446" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="447" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G447" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A48" r:id="rId1" xr:uid="{9AD3376E-B413-4678-A72A-CE864092C24B}"/>
+    <hyperlink ref="A46" r:id="rId1" xr:uid="{9AD3376E-B413-4678-A72A-CE864092C24B}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{3C38974D-A9D7-448F-B326-6287C2BE59B0}"/>
     <hyperlink ref="A3" r:id="rId3" xr:uid="{30863E05-E9AA-4FBC-A1A3-7396762B32CF}"/>
     <hyperlink ref="A4" r:id="rId4" xr:uid="{0555D538-2EF5-4DC7-81ED-2C9772EAA2AC}"/>
-    <hyperlink ref="A76" r:id="rId5" xr:uid="{9278788F-1DCB-4EF4-AA98-9A4CF64070B9}"/>
-    <hyperlink ref="A75" r:id="rId6" xr:uid="{2844140A-254D-4098-9CD9-1FDAC1693009}"/>
-    <hyperlink ref="A74" r:id="rId7" xr:uid="{5D908AFD-66CF-48D4-B602-C6F1B332A9FF}"/>
-    <hyperlink ref="A73" r:id="rId8" xr:uid="{F3EB05FB-0381-43C1-8F42-8928B315B982}"/>
-    <hyperlink ref="A72" r:id="rId9" xr:uid="{98984E02-BFDF-486A-BFA8-6D3B9DF045F6}"/>
-    <hyperlink ref="A71" r:id="rId10" xr:uid="{006DD930-C3C3-4E94-AC90-83D23ECD6850}"/>
-    <hyperlink ref="A68" r:id="rId11" xr:uid="{A26E5054-14F0-4836-8C1C-0B9787062CE0}"/>
-    <hyperlink ref="A67" r:id="rId12" xr:uid="{2668573E-BDE2-4F86-9288-A02D3977757F}"/>
-    <hyperlink ref="A65" r:id="rId13" xr:uid="{A1243D57-20FE-4DA3-93EF-92968212C323}"/>
-    <hyperlink ref="A64" r:id="rId14" xr:uid="{B178A11B-9E9E-48F4-9D45-71F719B86FA0}"/>
-    <hyperlink ref="A63" r:id="rId15" xr:uid="{6F337DDE-D24E-48FE-B274-737D7B1F3C6E}"/>
-    <hyperlink ref="A62" r:id="rId16" xr:uid="{B7C0B09B-7247-4788-A38B-CD21F6E0A833}"/>
-    <hyperlink ref="A60" r:id="rId17" xr:uid="{D123FC02-1A5F-49B6-833E-54B36FF7CD89}"/>
-    <hyperlink ref="A58" r:id="rId18" xr:uid="{AB9FF77C-F819-4819-A2C8-F61863E5ECAC}"/>
-    <hyperlink ref="A56" r:id="rId19" xr:uid="{EA3F6B5E-5EE9-4BFC-B8FE-E525424F3114}"/>
-    <hyperlink ref="A55" r:id="rId20" xr:uid="{CEF86BBA-1B0D-4713-937B-026F681EB32B}"/>
-    <hyperlink ref="A54" r:id="rId21" xr:uid="{5978B35E-F982-47B6-91CA-9766F7D2A0F5}"/>
-    <hyperlink ref="A53" r:id="rId22" xr:uid="{DB70101A-38EE-4B4A-A14A-731CD129D7D2}"/>
-    <hyperlink ref="A51" r:id="rId23" xr:uid="{0DF62B47-E388-4FB0-89DB-F84E895CD862}"/>
-    <hyperlink ref="A50" r:id="rId24" xr:uid="{1ADC068F-A0DF-485E-8E82-5FE601D6403F}"/>
-    <hyperlink ref="A49" r:id="rId25" xr:uid="{FA68AC9A-CE90-4B52-8C54-C08046E1AB88}"/>
-    <hyperlink ref="A46" r:id="rId26" xr:uid="{2FB4A02A-1314-4DF9-9CDF-3D5854095A11}"/>
-    <hyperlink ref="A44" r:id="rId27" display="Microcosm" xr:uid="{47E4C543-DD65-40F4-8877-15155A39E91C}"/>
-    <hyperlink ref="A43" r:id="rId28" xr:uid="{1071BE87-7071-45F5-BF3D-F1CE299CAF08}"/>
-    <hyperlink ref="A42" r:id="rId29" xr:uid="{987F8C39-C092-4525-82FF-C6D156C5FF4E}"/>
-    <hyperlink ref="A41" r:id="rId30" xr:uid="{B070C3A9-2141-4B19-BF27-B398BC0CA260}"/>
-    <hyperlink ref="A39" r:id="rId31" xr:uid="{AD8F3444-F974-4490-A2CE-D72C150379A6}"/>
-    <hyperlink ref="A38" r:id="rId32" xr:uid="{539B247F-9FE1-4DC9-BA1C-F422D0BE4FB1}"/>
+    <hyperlink ref="A73" r:id="rId5" xr:uid="{9278788F-1DCB-4EF4-AA98-9A4CF64070B9}"/>
+    <hyperlink ref="A72" r:id="rId6" xr:uid="{2844140A-254D-4098-9CD9-1FDAC1693009}"/>
+    <hyperlink ref="A71" r:id="rId7" xr:uid="{5D908AFD-66CF-48D4-B602-C6F1B332A9FF}"/>
+    <hyperlink ref="A70" r:id="rId8" xr:uid="{F3EB05FB-0381-43C1-8F42-8928B315B982}"/>
+    <hyperlink ref="A69" r:id="rId9" xr:uid="{98984E02-BFDF-486A-BFA8-6D3B9DF045F6}"/>
+    <hyperlink ref="A68" r:id="rId10" xr:uid="{006DD930-C3C3-4E94-AC90-83D23ECD6850}"/>
+    <hyperlink ref="A65" r:id="rId11" xr:uid="{A26E5054-14F0-4836-8C1C-0B9787062CE0}"/>
+    <hyperlink ref="A64" r:id="rId12" xr:uid="{2668573E-BDE2-4F86-9288-A02D3977757F}"/>
+    <hyperlink ref="A62" r:id="rId13" xr:uid="{A1243D57-20FE-4DA3-93EF-92968212C323}"/>
+    <hyperlink ref="A61" r:id="rId14" xr:uid="{B178A11B-9E9E-48F4-9D45-71F719B86FA0}"/>
+    <hyperlink ref="A60" r:id="rId15" xr:uid="{6F337DDE-D24E-48FE-B274-737D7B1F3C6E}"/>
+    <hyperlink ref="A59" r:id="rId16" xr:uid="{B7C0B09B-7247-4788-A38B-CD21F6E0A833}"/>
+    <hyperlink ref="A58" r:id="rId17" xr:uid="{D123FC02-1A5F-49B6-833E-54B36FF7CD89}"/>
+    <hyperlink ref="A56" r:id="rId18" xr:uid="{AB9FF77C-F819-4819-A2C8-F61863E5ECAC}"/>
+    <hyperlink ref="A54" r:id="rId19" xr:uid="{EA3F6B5E-5EE9-4BFC-B8FE-E525424F3114}"/>
+    <hyperlink ref="A53" r:id="rId20" xr:uid="{CEF86BBA-1B0D-4713-937B-026F681EB32B}"/>
+    <hyperlink ref="A52" r:id="rId21" xr:uid="{5978B35E-F982-47B6-91CA-9766F7D2A0F5}"/>
+    <hyperlink ref="A51" r:id="rId22" xr:uid="{DB70101A-38EE-4B4A-A14A-731CD129D7D2}"/>
+    <hyperlink ref="A49" r:id="rId23" xr:uid="{0DF62B47-E388-4FB0-89DB-F84E895CD862}"/>
+    <hyperlink ref="A48" r:id="rId24" xr:uid="{1ADC068F-A0DF-485E-8E82-5FE601D6403F}"/>
+    <hyperlink ref="A47" r:id="rId25" xr:uid="{FA68AC9A-CE90-4B52-8C54-C08046E1AB88}"/>
+    <hyperlink ref="A44" r:id="rId26" xr:uid="{2FB4A02A-1314-4DF9-9CDF-3D5854095A11}"/>
+    <hyperlink ref="A42" r:id="rId27" xr:uid="{47E4C543-DD65-40F4-8877-15155A39E91C}"/>
+    <hyperlink ref="A41" r:id="rId28" xr:uid="{1071BE87-7071-45F5-BF3D-F1CE299CAF08}"/>
+    <hyperlink ref="A40" r:id="rId29" xr:uid="{987F8C39-C092-4525-82FF-C6D156C5FF4E}"/>
+    <hyperlink ref="A39" r:id="rId30" xr:uid="{B070C3A9-2141-4B19-BF27-B398BC0CA260}"/>
+    <hyperlink ref="A37" r:id="rId31" xr:uid="{AD8F3444-F974-4490-A2CE-D72C150379A6}"/>
+    <hyperlink ref="A36" r:id="rId32" xr:uid="{539B247F-9FE1-4DC9-BA1C-F422D0BE4FB1}"/>
     <hyperlink ref="A34" r:id="rId33" xr:uid="{13E1AE0C-6285-4605-BC88-987DC6D8C72C}"/>
     <hyperlink ref="A33" r:id="rId34" xr:uid="{6660FFA3-EF90-46B2-9E92-FA340F79709C}"/>
     <hyperlink ref="A32" r:id="rId35" xr:uid="{8BF163D2-D2AE-4445-9A93-7546C05CF4DC}"/>
@@ -4279,11 +4277,17 @@
     <hyperlink ref="A7" r:id="rId57" xr:uid="{0F0C3D2D-C65E-42B1-884B-31D261D54696}"/>
     <hyperlink ref="A6" r:id="rId58" xr:uid="{EFF11699-C4B4-410F-A739-2602E91BB7A4}"/>
     <hyperlink ref="A5" r:id="rId59" xr:uid="{2E7A3AF1-B80C-4D12-9052-5E9C667F03AE}"/>
+    <hyperlink ref="A14" r:id="rId60" xr:uid="{2C7BD41E-11A6-4EE8-B366-2EF6A0F4F576}"/>
+    <hyperlink ref="A38" r:id="rId61" xr:uid="{D3024FFA-337E-4033-9AB9-EEA5C3808219}"/>
+    <hyperlink ref="A43" r:id="rId62" xr:uid="{E42B7800-EC66-4936-B8AF-FA517BBF9C0E}"/>
+    <hyperlink ref="A57" r:id="rId63" xr:uid="{D5F14801-3FD6-43C5-9790-FB44CB32C9A0}"/>
+    <hyperlink ref="A63" r:id="rId64" xr:uid="{30D15D1D-7848-44C9-8BA4-E68D099D30E6}"/>
+    <hyperlink ref="A66" r:id="rId65" xr:uid="{47235F79-1ECC-424B-97A4-926B7DF06831}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId60"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId66"/>
   <tableParts count="1">
-    <tablePart r:id="rId61"/>
+    <tablePart r:id="rId67"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>